<commit_message>
clean up graphs and code
</commit_message>
<xml_diff>
--- a/hw2_graphs.xlsx
+++ b/hw2_graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gafei/Documents/school/CSE674/hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE945FC-BEEC-F647-832E-D02C05227573}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB1834-74F3-9946-A5BA-EC017A4C3543}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{5E328D2E-C832-EF48-B045-116F90323F01}"/>
   </bookViews>
@@ -1132,6 +1132,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2387,6 +2449,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3642,6 +3766,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4894,6 +5080,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6146,6 +6394,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7400,6 +7703,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11513,8 +11871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E29745-71CA-F84C-A41D-FACD6E0F231B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11853,8 +12211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4D9519-3B2C-0E4C-8C70-E19C18C4B60F}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12188,8 +12546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64E76ED-9207-424D-A31F-A98E8F3FF0CD}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished readme.txt. Made excel sheet in landscape mode
</commit_message>
<xml_diff>
--- a/hw2_graphs.xlsx
+++ b/hw2_graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gafei/Documents/school/CSE674/hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB1834-74F3-9946-A5BA-EC017A4C3543}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC0F1F-009C-434A-8180-D007B7E016FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{5E328D2E-C832-EF48-B045-116F90323F01}"/>
   </bookViews>
@@ -3747,7 +3747,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -11347,8 +11346,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11871,8 +11870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E29745-71CA-F84C-A41D-FACD6E0F231B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12203,6 +12202,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -12211,8 +12211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4D9519-3B2C-0E4C-8C70-E19C18C4B60F}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12538,6 +12538,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -12546,8 +12547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64E76ED-9207-424D-A31F-A98E8F3FF0CD}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12877,6 +12878,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>